<commit_message>
creating .csv files for the data tables and changing repo structure
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/09f288fe3c2755fb/3b/ece356/simple_db_social_network/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:4000b_{AED0406B-BF3C-8146-BA40-C5450FA71DB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:4000b_{2C78BF34-55FA-9243-9029-1C020612483A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="10000" windowHeight="15640" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="People" sheetId="1" r:id="rId1"/>
@@ -3609,7 +3609,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+      <selection sqref="A1:F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5106,8 +5106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E449" zoomScale="99" workbookViewId="0">
-      <selection activeCell="G449" sqref="G449"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="99" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G1476"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5140,7 +5140,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -6336,7 +6336,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -8820,7 +8820,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>161</v>
       </c>
@@ -14087,7 +14087,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="391" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="391" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A391">
         <v>390</v>
       </c>
@@ -14340,7 +14340,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="402" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="402" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A402">
         <v>401</v>
       </c>
@@ -16364,7 +16364,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="490" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="490" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A490">
         <v>489</v>
       </c>
@@ -22598,7 +22598,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="761" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="761" spans="1:7" ht="187" x14ac:dyDescent="0.2">
       <c r="A761">
         <v>760</v>
       </c>
@@ -23955,7 +23955,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="820" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="820" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A820">
         <v>819</v>
       </c>
@@ -25059,7 +25059,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="868" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="868" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A868">
         <v>867</v>
       </c>
@@ -25220,7 +25220,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="875" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="875" spans="1:7" ht="187" x14ac:dyDescent="0.2">
       <c r="A875">
         <v>874</v>
       </c>
@@ -35786,7 +35786,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="1382" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1382" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A1382">
         <v>1381</v>
       </c>

</xml_diff>